<commit_message>
updated test data sheet
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/TestData.xlsx
+++ b/src/test/resources/testdata/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asha_\eclipse-workspace-api\RestassuredProject\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37CA05B2-3637-41DC-95AD-5E1C04807CEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C8FB303-721A-47CF-9900-30A234FAD39E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -120,10 +120,10 @@
     <t>validateDeletedCustomer</t>
   </si>
   <si>
-    <t>cus_N9DWJ6Ol4mIfS5</t>
-  </si>
-  <si>
-    <t>cus_N9DWzWgEU3E4QT</t>
+    <t>cus_N9vHRyiv9GsnhO</t>
+  </si>
+  <si>
+    <t>cus_N9vHDHWtVlR36c</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
updated test data sheet and listener
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/TestData.xlsx
+++ b/src/test/resources/testdata/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asha_\eclipse-workspace-api\RestassuredProject\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C8FB303-721A-47CF-9900-30A234FAD39E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F135D61C-B65D-4938-A741-EC801570755C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -120,10 +120,10 @@
     <t>validateDeletedCustomer</t>
   </si>
   <si>
-    <t>cus_N9vHRyiv9GsnhO</t>
-  </si>
-  <si>
-    <t>cus_N9vHDHWtVlR36c</t>
+    <t>cus_N9wDkXhr3jDaG4</t>
+  </si>
+  <si>
+    <t>cus_N9wDQ2uSnGUTFx</t>
   </si>
 </sst>
 </file>

</xml_diff>